<commit_message>
Arrumando a tabela colaboradores
</commit_message>
<xml_diff>
--- a/datatables/Colaboradores e Id.xlsx
+++ b/datatables/Colaboradores e Id.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" refMode="R1C1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -112,15 +112,9 @@
     <t>AMANDA BERNARDES</t>
   </si>
   <si>
-    <t>MICHELE MATTIDORF</t>
-  </si>
-  <si>
     <t>DANIELA FERNANDES</t>
   </si>
   <si>
-    <t>5eaaaf996310c300155bdae6</t>
-  </si>
-  <si>
     <t>5eaab2456310c300155bdd2b</t>
   </si>
   <si>
@@ -215,6 +209,12 @@
   </si>
   <si>
     <t>5eaabdfb6f443f00162e1e07</t>
+  </si>
+  <si>
+    <t>5eaab222c733400015fa33d8</t>
+  </si>
+  <si>
+    <t>MICHELE MATTIDORFF</t>
   </si>
 </sst>
 </file>
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,7 +609,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75">
@@ -617,7 +617,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75">
@@ -625,7 +625,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75">
@@ -633,7 +633,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75">
@@ -641,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75">
@@ -649,7 +649,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75">
@@ -657,7 +657,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75">
@@ -665,7 +665,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75">
@@ -673,7 +673,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -682,15 +682,15 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75">
@@ -698,7 +698,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -707,7 +707,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75">
@@ -715,7 +715,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75">
@@ -723,15 +723,15 @@
         <v>31</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75">
@@ -739,7 +739,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75">
@@ -747,7 +747,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75">
@@ -755,7 +755,7 @@
         <v>28</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75">
@@ -763,7 +763,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75">
@@ -771,7 +771,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75">
@@ -779,7 +779,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75">
@@ -787,7 +787,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75">
@@ -795,7 +795,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75">
@@ -803,7 +803,7 @@
         <v>18</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75">
@@ -811,7 +811,7 @@
         <v>19</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75">
@@ -819,7 +819,7 @@
         <v>20</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75">
@@ -827,7 +827,7 @@
         <v>21</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75">
@@ -835,7 +835,7 @@
         <v>23</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75">
@@ -843,7 +843,7 @@
         <v>22</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75">
@@ -851,7 +851,7 @@
         <v>25</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75">
@@ -859,7 +859,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75">
@@ -867,7 +867,7 @@
         <v>26</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>